<commit_message>
Judge page was added and changes were made, commit to update the branch
</commit_message>
<xml_diff>
--- a/models/uploads/data.xlsx
+++ b/models/uploads/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandhu/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC671FE-EA22-B143-93B2-4533882BBA08}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76304951-3421-9E4C-A321-8B7D3620EB1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16200" xr2:uid="{5FB357BF-69B0-F94A-ACF1-11078167B350}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
made some changes in index and added few more html pages and db functions
</commit_message>
<xml_diff>
--- a/models/uploads/data.xlsx
+++ b/models/uploads/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandhu/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC671FE-EA22-B143-93B2-4533882BBA08}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76304951-3421-9E4C-A321-8B7D3620EB1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16200" xr2:uid="{5FB357BF-69B0-F94A-ACF1-11078167B350}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C14" sqref="C14"/>
+      <selection activeCell="B15" sqref="B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
made changes on admin, index, and create comp page
</commit_message>
<xml_diff>
--- a/models/uploads/data.xlsx
+++ b/models/uploads/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandhu/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76304951-3421-9E4C-A321-8B7D3620EB1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC671FE-EA22-B143-93B2-4533882BBA08}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16200" xr2:uid="{5FB357BF-69B0-F94A-ACF1-11078167B350}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
added menu to the admin page
</commit_message>
<xml_diff>
--- a/models/uploads/data.xlsx
+++ b/models/uploads/data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/sandhu/Desktop/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76304951-3421-9E4C-A321-8B7D3620EB1A}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FC671FE-EA22-B143-93B2-4533882BBA08}" xr6:coauthVersionLast="32" xr6:coauthVersionMax="32" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="380" yWindow="460" windowWidth="28040" windowHeight="16200" xr2:uid="{5FB357BF-69B0-F94A-ACF1-11078167B350}"/>
   </bookViews>
@@ -467,7 +467,7 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B15" sqref="B15"/>
+      <selection activeCell="C14" sqref="C14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>